<commit_message>
Total Qty Stories Finished
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Dashboard</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>VP0911</t>
+  </si>
+  <si>
+    <t>https://qa.calcuquote.com/QAIdentity/</t>
   </si>
 </sst>
 </file>
@@ -525,7 +531,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -539,14 +545,15 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
     <col min="3" max="3" width="83" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
@@ -554,6 +561,9 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -672,7 +682,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" customHeight="1">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -680,7 +690,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" customHeight="1">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -688,7 +698,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" customHeight="1">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -696,7 +706,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" customHeight="1">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -704,7 +714,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" customHeight="1">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -712,7 +722,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" customHeight="1">
+    <row r="22" spans="1:3" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -720,7 +730,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" customHeight="1">
+    <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -728,7 +738,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" customHeight="1">
+    <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -736,7 +746,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" customHeight="1">
+    <row r="25" spans="1:3" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -744,7 +754,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" customHeight="1">
+    <row r="26" spans="1:3" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -752,7 +762,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" customHeight="1">
+    <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -760,7 +770,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" customHeight="1">
+    <row r="28" spans="1:3" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -768,20 +778,24 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" customHeight="1">
+    <row r="30" spans="1:3" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="C1" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B1" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Block API for Line Items
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>Dashboard</t>
   </si>
@@ -181,16 +181,22 @@
     <t>Enter Customer name:</t>
   </si>
   <si>
-    <t>tata</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>VP0911</t>
   </si>
   <si>
     <t>https://qa.calcuquote.com/QAIdentity/</t>
+  </si>
+  <si>
+    <t>https://app.calcuquote.com/Staging/</t>
+  </si>
+  <si>
+    <t>VP</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Tata</t>
   </si>
 </sst>
 </file>
@@ -531,7 +537,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -542,10 +548,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -556,7 +562,7 @@
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -564,10 +570,13 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -575,7 +584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -583,7 +592,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -591,7 +600,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -599,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -607,18 +616,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -626,7 +635,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
@@ -634,7 +643,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
@@ -642,7 +651,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -650,7 +659,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -658,7 +667,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -666,7 +675,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>19</v>
       </c>
@@ -674,7 +683,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -682,7 +691,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -690,7 +699,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -698,7 +707,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
@@ -706,7 +715,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
@@ -714,7 +723,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
@@ -722,7 +731,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15.75" customHeight="1">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
@@ -730,7 +739,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15.75" customHeight="1">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -738,7 +747,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15.75" customHeight="1">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
@@ -746,7 +755,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
         <v>29</v>
       </c>
@@ -754,7 +763,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
         <v>30</v>
       </c>
@@ -762,7 +771,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15.75" customHeight="1">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
@@ -770,7 +779,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
         <v>32</v>
       </c>
@@ -778,15 +787,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>57</v>
+      <c r="D30" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -794,8 +806,9 @@
     <hyperlink ref="B1" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="C1" r:id="rId3"/>
+    <hyperlink ref="D1" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>